<commit_message>
Atualização do script e README.md: inclusão de geração de combinações, ajuste de salvamento de arquivo na pasta correta e documentação aprimorada.
</commit_message>
<xml_diff>
--- a/Lotofácil/analise_lotofacil.xlsx
+++ b/Lotofácil/analise_lotofacil.xlsx
@@ -27016,7 +27016,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -27077,36 +27077,6 @@
       <c r="O2" t="n">
         <v>18</v>
       </c>
-      <c r="P2" t="n">
-        <v>22</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>19</v>
-      </c>
-      <c r="R2" t="n">
-        <v>21</v>
-      </c>
-      <c r="S2" t="n">
-        <v>15</v>
-      </c>
-      <c r="T2" t="n">
-        <v>7</v>
-      </c>
-      <c r="U2" t="n">
-        <v>17</v>
-      </c>
-      <c r="V2" t="n">
-        <v>23</v>
-      </c>
-      <c r="W2" t="n">
-        <v>6</v>
-      </c>
-      <c r="X2" t="n">
-        <v>8</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>16</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>